<commit_message>
pre split slurp between courses and instructors
</commit_message>
<xml_diff>
--- a/files/course_test/20220416_booth_faculty.xlsx
+++ b/files/course_test/20220416_booth_faculty.xlsx
@@ -2,20 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertyoung/Documents/repos/ruby-exercises/course_management/files/course_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039DD6E-5B92-3645-8214-EF0B4D0DA5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661D6ADA-FC0E-584C-B5E1-56635864D192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1380" windowWidth="19340" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1380" windowWidth="19340" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty &amp; Staff Directory" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6627,9 +6626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3453"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -41177,18 +41174,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>